<commit_message>
fix bait set and gene panels
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.34.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.34.balsamic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsdiazboada/Downloads/orderform1508.34/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsdiazboada/Documents/Clinical_Genomics/repos/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6DB05C-BF4B-D343-B5CC-3AAA2C22687C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5A8A39-2A00-7B4F-A3A3-1C700B372CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19400" yWindow="-21120" windowWidth="19000" windowHeight="21120" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="841">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -3604,6 +3604,9 @@
   </si>
   <si>
     <t>plate1</t>
+  </si>
+  <si>
+    <t>GMCKsolid</t>
   </si>
 </sst>
 </file>
@@ -5823,8 +5826,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15:S56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Y36" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="Z47" sqref="Z47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -34876,7 +34879,9 @@
       <c r="W38" s="136"/>
       <c r="X38" s="137"/>
       <c r="Y38" s="72"/>
-      <c r="Z38" s="87"/>
+      <c r="Z38" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA38" s="74"/>
       <c r="AB38" s="90"/>
       <c r="AC38" s="90"/>
@@ -34943,7 +34948,9 @@
       <c r="W39" s="136"/>
       <c r="X39" s="137"/>
       <c r="Y39" s="72"/>
-      <c r="Z39" s="87"/>
+      <c r="Z39" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA39" s="74"/>
       <c r="AB39" s="90"/>
       <c r="AC39" s="90"/>
@@ -36000,7 +36007,9 @@
       <c r="W40" s="136"/>
       <c r="X40" s="137"/>
       <c r="Y40" s="72"/>
-      <c r="Z40" s="87"/>
+      <c r="Z40" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA40" s="74"/>
       <c r="AB40" s="90"/>
       <c r="AC40" s="90"/>
@@ -37057,7 +37066,9 @@
       <c r="W41" s="136"/>
       <c r="X41" s="137"/>
       <c r="Y41" s="72"/>
-      <c r="Z41" s="87"/>
+      <c r="Z41" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA41" s="74"/>
       <c r="AB41" s="90"/>
       <c r="AC41" s="90"/>
@@ -38114,7 +38125,9 @@
       <c r="W42" s="136"/>
       <c r="X42" s="137"/>
       <c r="Y42" s="72"/>
-      <c r="Z42" s="87"/>
+      <c r="Z42" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA42" s="74"/>
       <c r="AB42" s="90"/>
       <c r="AC42" s="90"/>
@@ -39171,7 +39184,9 @@
       <c r="W43" s="136"/>
       <c r="X43" s="137"/>
       <c r="Y43" s="72"/>
-      <c r="Z43" s="87"/>
+      <c r="Z43" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA43" s="74"/>
       <c r="AB43" s="90"/>
       <c r="AC43" s="90"/>
@@ -40228,7 +40243,9 @@
       <c r="W44" s="136"/>
       <c r="X44" s="137"/>
       <c r="Y44" s="72"/>
-      <c r="Z44" s="87"/>
+      <c r="Z44" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA44" s="74"/>
       <c r="AB44" s="90"/>
       <c r="AC44" s="90"/>
@@ -41285,7 +41302,9 @@
       <c r="W45" s="136"/>
       <c r="X45" s="137"/>
       <c r="Y45" s="72"/>
-      <c r="Z45" s="87"/>
+      <c r="Z45" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA45" s="74"/>
       <c r="AB45" s="90"/>
       <c r="AC45" s="90"/>
@@ -42342,7 +42361,9 @@
       <c r="W46" s="136"/>
       <c r="X46" s="137"/>
       <c r="Y46" s="72"/>
-      <c r="Z46" s="87"/>
+      <c r="Z46" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA46" s="74"/>
       <c r="AB46" s="90"/>
       <c r="AC46" s="90"/>
@@ -43399,7 +43420,9 @@
       <c r="W47" s="136"/>
       <c r="X47" s="137"/>
       <c r="Y47" s="72"/>
-      <c r="Z47" s="87"/>
+      <c r="Z47" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA47" s="74"/>
       <c r="AB47" s="90"/>
       <c r="AC47" s="90"/>
@@ -44456,7 +44479,9 @@
       <c r="W48" s="136"/>
       <c r="X48" s="137"/>
       <c r="Y48" s="72"/>
-      <c r="Z48" s="87"/>
+      <c r="Z48" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA48" s="74"/>
       <c r="AB48" s="90"/>
       <c r="AC48" s="90"/>
@@ -45513,7 +45538,9 @@
       <c r="W49" s="136"/>
       <c r="X49" s="137"/>
       <c r="Y49" s="72"/>
-      <c r="Z49" s="87"/>
+      <c r="Z49" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA49" s="74"/>
       <c r="AB49" s="90"/>
       <c r="AC49" s="90"/>
@@ -46571,7 +46598,9 @@
       <c r="W50" s="136"/>
       <c r="X50" s="137"/>
       <c r="Y50" s="72"/>
-      <c r="Z50" s="87"/>
+      <c r="Z50" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA50" s="74"/>
       <c r="AB50" s="90"/>
       <c r="AC50" s="90"/>
@@ -46638,7 +46667,9 @@
       <c r="W51" s="136"/>
       <c r="X51" s="137"/>
       <c r="Y51" s="72"/>
-      <c r="Z51" s="87"/>
+      <c r="Z51" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA51" s="74"/>
       <c r="AB51" s="90"/>
       <c r="AC51" s="90"/>
@@ -47695,7 +47726,9 @@
       <c r="W52" s="136"/>
       <c r="X52" s="137"/>
       <c r="Y52" s="72"/>
-      <c r="Z52" s="87"/>
+      <c r="Z52" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA52" s="74"/>
       <c r="AB52" s="90"/>
       <c r="AC52" s="90"/>
@@ -48752,7 +48785,9 @@
       <c r="W53" s="136"/>
       <c r="X53" s="137"/>
       <c r="Y53" s="72"/>
-      <c r="Z53" s="87"/>
+      <c r="Z53" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA53" s="74"/>
       <c r="AB53" s="90"/>
       <c r="AC53" s="90"/>
@@ -49809,7 +49844,9 @@
       <c r="W54" s="136"/>
       <c r="X54" s="137"/>
       <c r="Y54" s="72"/>
-      <c r="Z54" s="87"/>
+      <c r="Z54" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA54" s="74"/>
       <c r="AB54" s="90"/>
       <c r="AC54" s="90"/>
@@ -50866,7 +50903,9 @@
       <c r="W55" s="136"/>
       <c r="X55" s="137"/>
       <c r="Y55" s="72"/>
-      <c r="Z55" s="87"/>
+      <c r="Z55" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA55" s="74"/>
       <c r="AB55" s="90"/>
       <c r="AC55" s="90"/>
@@ -51923,7 +51962,9 @@
       <c r="W56" s="136"/>
       <c r="X56" s="137"/>
       <c r="Y56" s="72"/>
-      <c r="Z56" s="87"/>
+      <c r="Z56" s="87" t="s">
+        <v>840</v>
+      </c>
       <c r="AA56" s="74"/>
       <c r="AB56" s="90"/>
       <c r="AC56" s="90"/>

</xml_diff>